<commit_message>
Last changes after checking in search
</commit_message>
<xml_diff>
--- a/1_Search/Summary.xlsx
+++ b/1_Search/Summary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\_General\DoctoradoIndustrial2022\Publicaciones\METAANALISIS\Documentos\1_Searches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\metaanalysisT2D\1_Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64512E0A-00CF-4902-ADDA-486D9D65658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A6679-0EB0-4F6D-8CDF-E1229AD36FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{80FFF016-06F5-4035-8E12-139E4C93443F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{80FFF016-06F5-4035-8E12-139E4C93443F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Preliminary search" sheetId="1" r:id="rId1"/>
-    <sheet name="Main search" sheetId="2" r:id="rId2"/>
+    <sheet name="README" sheetId="3" r:id="rId1"/>
+    <sheet name="Preliminary search" sheetId="1" r:id="rId2"/>
+    <sheet name="Main search" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Date of search</t>
   </si>
@@ -94,18 +95,51 @@
 AND 
 ("biomarker*" [Title/Abstract] OR "significant protein" [Title/Abstract] OR "differential expressed protein" [Title/Abstract] OR "DE protein" [Title/Abstract] OR "protein biomarker" [Title/Abstract] OR "upregul* protein*" [Title/Abstract] OR "downregul* protein*" [Title/Abstract] OR "signific* higher protein*" [Title/Abstract] OR "signific* increased protein*" [Title/Abstract] OR "signific* lower protein*" [Title/Abstract] OR "signific* reduced protein*" [Title/Abstract] OR "express* protein*" [Title/Abstract] OR "protein* express*" [Title/Abstract] OR "protein* level*" [Title/Abstract] OR "protein* marker*" [Title/Abstract])</t>
   </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Preliminary search</t>
+  </si>
+  <si>
+    <t>Detailed description of initial search regarding equation, dates, aditional options and number of results retrieved in each of the databases</t>
+  </si>
+  <si>
+    <t>Main search</t>
+  </si>
+  <si>
+    <t>Detailed description of final search regarding refined equation, dates, aditional options and number of results retrieved in each of the databases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -139,6 +173,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,12 +496,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB01D007-38BA-4720-ACAD-873C51B1952A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="87.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25DBFD4-07D3-48F9-93EF-09F12010C9F3}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -543,13 +631,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E894626F-5C64-4BC9-9B8E-9BB7884624D3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>